<commit_message>
added wordnet to normalize words before comparing and implemented word2vec for labels representation. calculated cosine similarity, precision, recall and f1
</commit_message>
<xml_diff>
--- a/input/ground_truth_cluster_labels.xlsx
+++ b/input/ground_truth_cluster_labels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdica\Desktop\TESI\CODICE_TESI\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdica\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC349D50-AC37-4A1D-9D4C-E0AFCA9184BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F82FB414-5E35-4F0D-B681-EA79A6EFE17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9435" yWindow="2235" windowWidth="18495" windowHeight="13245" xr2:uid="{668BE5BF-477E-4EA6-A373-4C5CC5A4E637}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{668BE5BF-477E-4EA6-A373-4C5CC5A4E637}"/>
   </bookViews>
   <sheets>
     <sheet name="ground_truth_cluster_labels" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Cluster</t>
   </si>
@@ -28,111 +28,42 @@
     <t>Label</t>
   </si>
   <si>
-    <t xml:space="preserve">isolette single sensor temperature alarm </t>
-  </si>
-  <si>
-    <t>Drone rendezvous control system considering currX currY accX accY velX velY</t>
-  </si>
-  <si>
     <t>aaspe security system</t>
   </si>
   <si>
-    <t>translator device for abstract and missing data, smart parking driver system</t>
-  </si>
-  <si>
-    <t>position control system, CMPare comparing customer service for product and seller, vehicle toll collection payment system, mece learning app system that get req send reply, xdl to aadl open tool</t>
-  </si>
-  <si>
-    <t>power manager system with sensorin and sensorout</t>
-  </si>
-  <si>
-    <t>security system</t>
-  </si>
-  <si>
-    <t>test system for bus access</t>
-  </si>
-  <si>
-    <t>security system integration for datain and dataout, UAVnetwork for structural deformation inspection using drones</t>
-  </si>
-  <si>
     <t>structural deformation inspection using drones</t>
   </si>
   <si>
-    <t>ocarina outp inp</t>
-  </si>
-  <si>
-    <t>communication architecture for network and system management</t>
-  </si>
-  <si>
     <t>aps communication architecture using lidar and radar</t>
   </si>
   <si>
-    <t>integration model for merge models</t>
-  </si>
-  <si>
     <t>smart home sensor system</t>
   </si>
   <si>
-    <t>paparazzi ariborne system, vending machine system, car collision detection system</t>
-  </si>
-  <si>
-    <t>self driving car integration system for speed distance brake and obstacle managing, humidifier and dehumidifier managing system</t>
-  </si>
-  <si>
     <t>pulseox forwarding system, train movement authority controller, flowlatencysampledata application system</t>
   </si>
   <si>
-    <t>security failure datain dataout, isolette dual sensor temp alarm system, communication architecture dataport</t>
-  </si>
-  <si>
     <t>isolette temp monitoring system with alarm, communication architecture for gnss security, aviate control altitude latitude longitude distance speed, tank pressurized valve switch</t>
   </si>
   <si>
     <t>smartparking system for vehicle considering space occupancy and capacity, aviation temperature controller sensor, isolette temperature sensor monitor heat with thermostat and alarm, aps communication architecture</t>
   </si>
   <si>
-    <t>aviation supervisor for altitude gcas tcas latitude longitude, car cruise control for speed velocity and throttle, blocks memory management using bus</t>
-  </si>
-  <si>
-    <t>radiation pressure sensor shutdown system, temp controller heater and cooler, delivery drone system using gps navigation radio,  learning system master slave with write read update sync operations</t>
-  </si>
-  <si>
     <t>smart home remote controller with clients sender and reciever, traffic light signal sensor to switch color</t>
   </si>
   <si>
     <t>aaspe security timing requirements</t>
   </si>
   <si>
-    <t>tasklibrary map view</t>
-  </si>
-  <si>
-    <t>scenario producer consumer implementation</t>
-  </si>
-  <si>
     <t>polyorb scenario types implementation</t>
   </si>
   <si>
-    <t>flight management scenario implementation</t>
-  </si>
-  <si>
-    <t>vehicle toll collection payment administation system, isolette heat control and monitor system through sensor thermostat and alarm, military radar contact system for number of target threath position and status, smart parking vehicle system, collision detection and avoidance system</t>
-  </si>
-  <si>
     <t>resourcebudgets sensor monitoring hardware power for cpu pci and ram, pcb hardware maintenance system, networking hardware model, automotive car hardware integration cellullar or router for internet access</t>
   </si>
   <si>
-    <t>issue182 test impl</t>
-  </si>
-  <si>
-    <t>ocarina system</t>
-  </si>
-  <si>
     <t>iplprojects edge map</t>
   </si>
   <si>
-    <t>polyorb ping scenario impl</t>
-  </si>
-  <si>
     <t>polyorb rma scenario impl</t>
   </si>
   <si>
@@ -145,19 +76,85 @@
     <t>ksu isolette single and dual sensor</t>
   </si>
   <si>
-    <t>polyorb rma impl test, ocarina rma, sunseeker control system</t>
-  </si>
-  <si>
     <t>ping pong event system node</t>
   </si>
   <si>
-    <t>pacemaker for heart rate monitoring model, radio and gps system, coffee machine system impl, flightcontroller example impl, groundstation example impl</t>
-  </si>
-  <si>
-    <t>pca management system for medical drug infusion, isolette temperature sensor for heat source, gps satellite position observation, ocarina vehicle speed monitor</t>
-  </si>
-  <si>
     <t>adiru event monitoring alarm system, dca resourcebudget app with sensorin and actuatorout, security algorithm system for crypto, mine pump monitoring software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isolette single sensor thermostat temperature alarm </t>
+  </si>
+  <si>
+    <t>security failure datain dataout, isolette dual sensor temp alarm, communication aps architecture dataport</t>
+  </si>
+  <si>
+    <t>aviation supervisor for altitude gcas tcas latitude longitude, car cruisecontrol for speed velocity and throttle, blocks memory management using bus</t>
+  </si>
+  <si>
+    <t>thesis drone rendezvous control system considering currX currY accX accY velX velY</t>
+  </si>
+  <si>
+    <t>radiation pressure sensor shutdown, temp controller heater and cooler, delivery drone system using gps navigation radio,  learning system master slave with write read update sync operations</t>
+  </si>
+  <si>
+    <t>iplprojects tasklibrary map view</t>
+  </si>
+  <si>
+    <t>scenario producer consumer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translator device for abstract and missing data, smartparkingsystem driver </t>
+  </si>
+  <si>
+    <t>flight management scenario</t>
+  </si>
+  <si>
+    <t>position control system, cmpare comparing learning model customer service for product and seller, vehicle toll collection payment model, mece learning app system that get req send reply</t>
+  </si>
+  <si>
+    <t>vehicle toll collection payment administation system, isolette heat control and monitor system through temperature sensor thermostat and alarm, military radar contact system of target threath position and weapon status, smart parking vehicle system, collision detection and avoidance system</t>
+  </si>
+  <si>
+    <t>power manager system with sensorin sensorout actuatorout</t>
+  </si>
+  <si>
+    <t>test impl for bus access</t>
+  </si>
+  <si>
+    <t>aaspe security system integration for datain and dataout, flying structural deformation inspection using drones</t>
+  </si>
+  <si>
+    <t>ocarina issue test outp inp</t>
+  </si>
+  <si>
+    <t>communication architecture for networking and system management</t>
+  </si>
+  <si>
+    <t>polyorb ping scenario</t>
+  </si>
+  <si>
+    <t>ocarina issue test impl</t>
+  </si>
+  <si>
+    <t>ocarina</t>
+  </si>
+  <si>
+    <t>polyorb rma impl test, ocarina rma, sunseekercontrolsystem</t>
+  </si>
+  <si>
+    <t>integration model for merged models</t>
+  </si>
+  <si>
+    <t>paparazzo ariborne system, vending machine system, car collision detection sensor avoidable unavoidable</t>
+  </si>
+  <si>
+    <t>self driving car integration system for speed distance brake and obstacle managing, humidifier and dehumidifier managing sensor</t>
+  </si>
+  <si>
+    <t>pacemaker for heart rate monitoring model, radio and gps system, coffeemachine system impl, flightcontroller example impl, groundstation example impl</t>
+  </si>
+  <si>
+    <t>pca management system for patient drug infusion, isolette temperature sensor for heat source, gps satellite position observation, ocarina vehicle speed monitor</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +998,7 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1022,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1030,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -1038,7 +1035,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -1046,7 +1043,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -1054,7 +1051,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -1062,7 +1059,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -1078,7 +1075,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
@@ -1086,7 +1083,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
@@ -1094,7 +1091,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -1102,7 +1099,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -1110,7 +1107,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
@@ -1118,7 +1115,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -1126,7 +1123,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -1134,7 +1131,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -1142,7 +1139,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -1150,7 +1147,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
@@ -1158,7 +1155,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
@@ -1166,7 +1163,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
@@ -1174,7 +1171,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
@@ -1182,7 +1179,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
@@ -1190,7 +1187,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
@@ -1198,7 +1195,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
@@ -1206,7 +1203,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
@@ -1214,7 +1211,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
@@ -1222,7 +1219,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
@@ -1230,7 +1227,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
@@ -1246,7 +1243,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
@@ -1254,7 +1251,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
@@ -1262,7 +1259,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
@@ -1270,7 +1267,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
@@ -1278,7 +1275,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
@@ -1286,7 +1283,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
@@ -1294,7 +1291,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
@@ -1302,7 +1299,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
@@ -1310,7 +1307,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
@@ -1318,7 +1315,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
@@ -1326,7 +1323,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
@@ -1334,7 +1331,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
@@ -1350,7 +1347,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
@@ -1366,7 +1363,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>